<commit_message>
working on Promo image using helper class
</commit_message>
<xml_diff>
--- a/test-data/promoimage-data.xlsx
+++ b/test-data/promoimage-data.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6763D9B6-6B46-4C7B-9D9A-285D06A890A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665B9BEC-AA85-4D62-ABF3-785022DA4637}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="2760" windowWidth="14925" windowHeight="5460" activeTab="1" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
+    <workbookView xWindow="4280" yWindow="2760" windowWidth="14920" windowHeight="5460" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
   </bookViews>
   <sheets>
-    <sheet name="pages_with_promoimage" sheetId="1" r:id="rId1"/>
-    <sheet name="pages_with_noleadimage" sheetId="5" r:id="rId2"/>
+    <sheet name="pages_with_promo+leadimage" sheetId="1" r:id="rId1"/>
+    <sheet name="List_with_promo+leadimage" sheetId="7" r:id="rId2"/>
+    <sheet name="List_with_lead_nopromoimage" sheetId="5" r:id="rId3"/>
+    <sheet name="page_with_nopromoimage" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>path</t>
   </si>
@@ -43,45 +45,9 @@
     <t>English</t>
   </si>
   <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>espanol/cancer/sobrellevar/sentimientos/hoja-informativa-estres</t>
-  </si>
-  <si>
-    <t>Blog Page</t>
-  </si>
-  <si>
-    <t>Cancer Center</t>
-  </si>
-  <si>
-    <t>Biography</t>
-  </si>
-  <si>
-    <t>about-cancer/coping/feelings/relaxation/stress-fact-sheet</t>
-  </si>
-  <si>
-    <t>test/no-lead-img</t>
-  </si>
-  <si>
-    <t>about-cancer/coping/feelings/test-biography</t>
-  </si>
-  <si>
-    <t>about-cancer/coping/feelings/test-cancer-center</t>
-  </si>
-  <si>
-    <t>research/key-initiatives/ras/ras-central/blog/2017/ras-dependent</t>
-  </si>
-  <si>
-    <t>Reconstruction</t>
-  </si>
-  <si>
     <t>Mini Landing Page</t>
   </si>
   <si>
-    <t>test/test-mini-promo</t>
-  </si>
-  <si>
     <t>Feature card</t>
   </si>
   <si>
@@ -97,13 +63,28 @@
     <t>Promo Alt text</t>
   </si>
   <si>
-    <t>/sites/default/files/styles/cgov_featured/public/2019-05/promo-placeholder-featured.png?itok=38OdaiPb</t>
-  </si>
-  <si>
     <t>Promo Placeholder</t>
   </si>
   <si>
-    <t>/sites/default/files/styles/cgov_featured/public/2019-05/old-man-smiling-with-doctor-article.jpg?h=6a76169e&amp;itok=FOK2YVah</t>
+    <t>research/key-initiatives</t>
+  </si>
+  <si>
+    <t>test/mini-landing/li-title-desc-img</t>
+  </si>
+  <si>
+    <t>about-cancer/coping</t>
+  </si>
+  <si>
+    <t>/about-nci/organization/ccct</t>
+  </si>
+  <si>
+    <t>/sites/default/files/styles/cgov_featured/public/2019-05/sad-woman-looking-out-window-feature.jpg?itok=wRPdOias</t>
+  </si>
+  <si>
+    <t>pets</t>
+  </si>
+  <si>
+    <t>/sites/default/files/styles/cgov_featured/public/2019-05/pet_zedd_happy.jpg?h=62addaa4&amp;itok=ovYp0yzC</t>
   </si>
 </sst>
 </file>
@@ -458,26 +439,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABDEF67-3BF3-604C-97A8-A43819B8E79D}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.75" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="23.125" customWidth="1"/>
-    <col min="6" max="6" width="18.875" customWidth="1"/>
-    <col min="7" max="7" width="31.375" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.58203125" customWidth="1"/>
+    <col min="5" max="5" width="23.08203125" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="86.75" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="34.125" customWidth="1"/>
+    <col min="9" max="9" width="34.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,27 +469,27 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -516,17 +497,19 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -535,21 +518,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26668E1C-E236-40F0-B5CF-1CC4E870A494}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043CBC06-B59A-468B-AF7A-85104B5D0776}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="66.375" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.58203125" customWidth="1"/>
+    <col min="5" max="5" width="23.08203125" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="86.75" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="34.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,10 +548,67 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26668E1C-E236-40F0-B5CF-1CC4E870A494}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -571,58 +617,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCA25E4-705C-4931-8A49-5B62B1C757C6}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="15.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>